<commit_message>
post git 4) LocalRepostory 작업파일 관리하기까지 완료
</commit_message>
<xml_diff>
--- a/_posts/git/2021/Git명령어.xlsx
+++ b/_posts/git/2021/Git명령어.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git-blog\Jjae-Jjae.github.io\_posts\git\2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047DBB79-406F-4E94-9B71-90AEA7C66A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B0C460-6965-457F-8A52-E2F67BE2E72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트 1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>$ git init</t>
   </si>
   <si>
-    <t>.git 하위 디렉토리 생성(폴더를 만든 후, 그 안에서 명령 실행 =&gt; 새로운 git저장소 생성)</t>
-  </si>
-  <si>
     <t>$ git clone &lt;https:.. URL&gt;</t>
   </si>
   <si>
@@ -46,9 +43,6 @@
     <t>$ git status</t>
   </si>
   <si>
-    <t>파일 상태 확인</t>
-  </si>
-  <si>
     <t>$ git branch</t>
   </si>
   <si>
@@ -82,18 +76,6 @@
     <t>$ git commit -a -m "[메시지명]"</t>
   </si>
   <si>
-    <t> 메시지 [메시지명]을 붙여서 스테이징과 커밋을 동시에 진행</t>
-  </si>
-  <si>
-    <t>커밋 메시지 [메시지명]을 붙여 커밋</t>
-  </si>
-  <si>
-    <t>커밋 내역 확인</t>
-  </si>
-  <si>
-    <t>한줄로 표기하기</t>
-  </si>
-  <si>
     <t>특정 커밋 내역 확인</t>
   </si>
   <si>
@@ -130,30 +112,15 @@
     <t>$ git reset --mixed [커밋ID]</t>
   </si>
   <si>
-    <t>$ git reset --soft [커밋ID]</t>
-  </si>
-  <si>
-    <t>$ git revert [커밋 해시]</t>
-  </si>
-  <si>
     <t>$ git commit --amend</t>
   </si>
   <si>
-    <t>: 최신 커밋 수정( 수정할 내용을 add를 통해 스테이징에 올려놔야함</t>
-  </si>
-  <si>
     <t>$ git log --oneline</t>
   </si>
   <si>
     <t>$ ​git log --branches --grap</t>
   </si>
   <si>
-    <t>커밋 로그에 각 브랜치의 커밋을 그래프로 표시</t>
-  </si>
-  <si>
-    <t>한줄로 표기하기(id 6자리만 출력됨)</t>
-  </si>
-  <si>
     <t>$ git merge [브랜치명]</t>
   </si>
   <si>
@@ -277,9 +244,6 @@
     <t>$ git stash pop</t>
   </si>
   <si>
-    <t>git config alias.[별명] '원하는 명령어'</t>
-  </si>
-  <si>
     <t>2) tag 설정 하기</t>
   </si>
   <si>
@@ -293,9 +257,6 @@
   </si>
   <si>
     <t>[원격저장소명]에 저장된 git프로젝트의 현 상태를 다운로드</t>
-  </si>
-  <si>
-    <t>) 지정한 커밋 해시의 변경 이력을 취소 (작업내용 log에 남음</t>
   </si>
   <si>
     <t>7) 보관한 내용을 적용 {n}(n번쨰 )</t>
@@ -360,10 +321,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>선택된 파일중 변경된 내용을 Index에 Staging함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$ git add &lt;파일경로&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -377,18 +334,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>파일 경로 내에 있는 파일만 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파일평 파일만 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모든파일 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$ git log --pretty=oneline</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -401,10 +346,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$ git reset --옵션 [커밋 해시]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$ git merge [브랜치명]--edit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -414,6 +355,113 @@
   </si>
   <si>
     <t>5) 작업 트리의 수정 내용 stash(Commit이 아닌 임시저장소)에 따로 보관하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 폴더를 Local Repository로 지정(폴더안에 .git폴더 생성됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경된 파일 목록 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택된 목록중 변경된 내용을 Index에 Staging함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 경로 내 변경된 내용을 Index에 Staging함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당파일 변경 내용을 Index에 Staging함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든파일의 변경된 내용을 Index에 Staging함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커밋 메시지 [메시지명]을 붙여 commit 진행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커밋 메시지를 붙여Staging과 commit을 동시에 진행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최근 커밋 수정
+(수정할 내용을 add를 통해 스테이징에 올려논뒤 진행해야함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커밋 내역 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커밋 내역 한줄로 표기하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커밋 내역 한줄로 표기하기(id를 6자리만 출력됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커밋 로그에 각 브랜치의 커밋을 그래프로 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ git reset --[옵션] [커밋 해시]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ git reset --soft [커밋ID]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지정한 커밋 해시의 변경 이력을 취소 (작업내용 log에 남음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config alias.[별명] '원하는 명령어'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ git revert [커밋 해시]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>새로운 브랜치를 만들고 stash된 내용을 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>pop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>합니다. </t>
+    </r>
+  </si>
+  <si>
+    <t>git stash clear:</t>
+  </si>
+  <si>
+    <t>모든 임시 변경사항(stash)을 삭제</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ git stash branch new-branch </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -421,7 +469,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -439,6 +487,33 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="나눔고딕"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -472,7 +547,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -487,6 +562,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,615 +746,631 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="46" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.75" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" style="2" customWidth="1"/>
-    <col min="6" max="6" width="62.85546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="62.875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="25.5">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="25.5">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="25.5">
       <c r="A9" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="E11"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E21"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E23"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E24"/>
       <c r="F24"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E25"/>
       <c r="F25"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E26"/>
       <c r="F26"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="E27"/>
       <c r="F27"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E28"/>
       <c r="F28"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E29"/>
       <c r="F29"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E30"/>
       <c r="F30"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E31"/>
       <c r="F31"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E32"/>
       <c r="F32"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E33"/>
       <c r="F33"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E34"/>
       <c r="F34"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E35"/>
       <c r="F35"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="E36"/>
       <c r="F36"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E37"/>
       <c r="F37"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="C42" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="C43" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="19.5">
+      <c r="C44" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="21.75">
+      <c r="C45" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>